<commit_message>
[EDIT] change sla employee
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_sla_employee.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_sla_employee.xlsx
@@ -393,8 +393,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="5" width="21.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="21.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="8" width="21.31"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="22" style="8" width="21.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="8" width="21.31"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="22" style="8" width="21.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="8" width="21.31"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>